<commit_message>
Created POM Class for Reviews Page					Created Test Class for Reviews Page					Created Abstract method for Reviews					Created Repository for Reviews
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{DA46DCB9-2D8E-4950-AF63-19854478272C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{D40E50A7-6A6E-4625-8DAD-5FCA498AEBEA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
+    <workbookView activeTab="4" windowHeight="10920" windowWidth="20490" xWindow="0" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
     <sheet name="Zoom" r:id="rId2" sheetId="2"/>
     <sheet name="PDF" r:id="rId3" sheetId="3"/>
+    <sheet name="SA_Filters" r:id="rId4" sheetId="4"/>
+    <sheet name="SA_Advanced_Filters" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -78,6 +80,48 @@
   </si>
   <si>
     <t>AE</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Owner Response</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Sentiment</t>
+  </si>
+  <si>
+    <t>Sentiment Category</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Atmosphere</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>manage</t>
   </si>
 </sst>
 </file>
@@ -85,7 +129,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +142,14 @@
       <color rgb="FF222222"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,11 +172,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -444,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +561,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,16 +570,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -582,22 +635,22 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+      <selection activeCell="A2" sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -626,4 +679,143 @@
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" r="1" s="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated highcharts methods for TSEE Reports
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{D40E50A7-6A6E-4625-8DAD-5FCA498AEBEA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{531628FA-8206-4504-805C-EF008F924D8B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView activeTab="4" windowHeight="10920" windowWidth="20490" xWindow="0" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="0"/>
+    <workbookView windowHeight="10920" windowWidth="20490" xWindow="0" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
@@ -79,9 +79,6 @@
     <t>November</t>
   </si>
   <si>
-    <t>AE</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>manage</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +538,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -751,7 +751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -769,49 +769,49 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPdated Code for TSEE and Social
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{ED7C3EBC-92AE-4C8B-92C3-AAA12E1D6E57}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{D806ED13-FC59-432A-81D7-108FB05B4B20}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="10920" windowWidth="20445" xWindow="45" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="0"/>
+    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
-    <sheet name="Zoom" r:id="rId2" sheetId="2"/>
-    <sheet name="PDF" r:id="rId3" sheetId="3"/>
-    <sheet name="SA_Filters" r:id="rId4" sheetId="4"/>
-    <sheet name="SA_Advanced_Filters" r:id="rId5" sheetId="5"/>
+    <sheet name="Sheet1" r:id="rId2" sheetId="6"/>
+    <sheet name="Zoom" r:id="rId3" sheetId="2"/>
+    <sheet name="PDF" r:id="rId4" sheetId="3"/>
+    <sheet name="SA_Filters" r:id="rId5" sheetId="4"/>
+    <sheet name="SA_Advanced_Filters" r:id="rId6" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -116,6 +117,18 @@
   </si>
   <si>
     <t>Good</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>The Little Beet, 19501 Biscayne Blvd, Treats Food Hall, Floor 3, 33180, +1 305-359-5808</t>
   </si>
 </sst>
 </file>
@@ -492,16 +505,16 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
     <col min="3" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="66.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -528,19 +541,19 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -551,6 +564,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -624,7 +670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -675,7 +721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -741,7 +787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
   <dimension ref="A1:J2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Working on the ROI part
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,37 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abinaya\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{C7C9D68B-5280-4E5F-8A91-B69F55881021}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{8BC30246-6FCF-4FB6-97CC-80A9C43B41E3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
+    <workbookView activeTab="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" r:id="rId2" sheetId="2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -67,6 +62,12 @@
   </si>
   <si>
     <t>US</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -74,7 +75,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +88,12 @@
       <color rgb="FF222222"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF393939"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,9 +116,10 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -428,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,4 +494,68 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF188180-7FBA-422A-8B4F-79B4DFA3F3C5}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="84.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Duplicate Management Code
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5D1606-52F2-41B4-AD6D-1DB28716CAB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC7C5AB-E757-4143-A533-BA23B23672B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -141,14 +141,17 @@
     <t>+1 610-488-2411</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/?q=place_id:ChIJMQ6lFrfW1IkRFe1flYsZ06A</t>
+    <t>https://www.google.com/maps/place/?q=place_id:ChIJLdD4Ikv1xokRXCXMOatucy4</t>
+  </si>
+  <si>
+    <t>Action Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +169,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -188,20 +199,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -577,32 +591,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -658,16 +679,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -729,16 +750,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Changes made by Aneesh
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aneeshc\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC7C5AB-E757-4143-A533-BA23B23672B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{B1B9883B-8408-4C7B-9A47-C46A7D0902DB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}"/>
+    <workbookView activeTab="5" windowHeight="15840" windowWidth="29040" xWindow="20370" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="TPSEE" sheetId="1" r:id="rId1"/>
-    <sheet name="Duplicate_Management" sheetId="7" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
-    <sheet name="Zoom" sheetId="2" r:id="rId4"/>
-    <sheet name="PDF" sheetId="3" r:id="rId5"/>
-    <sheet name="SA_Filters" sheetId="4" r:id="rId6"/>
-    <sheet name="SA_Advanced_Filters" sheetId="5" r:id="rId7"/>
+    <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
+    <sheet name="Display_Review" r:id="rId2" sheetId="9"/>
+    <sheet name="Bing" r:id="rId3" sheetId="8"/>
+    <sheet name="Duplicate_Management" r:id="rId4" sheetId="7"/>
+    <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
+    <sheet name="Zoom" r:id="rId6" sheetId="2"/>
+    <sheet name="PDF" r:id="rId7" sheetId="3"/>
+    <sheet name="SA_Filters" r:id="rId8" sheetId="4"/>
+    <sheet name="SA_Advanced_Filters" r:id="rId9" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="44">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -75,12 +77,6 @@
     <t>Year_YYYY</t>
   </si>
   <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>November</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -145,12 +141,37 @@
   </si>
   <si>
     <t>Action Value</t>
+  </si>
+  <si>
+    <t>except GMB , Face book , Bing</t>
+  </si>
+  <si>
+    <t>SWOOP_Create_One</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>The Little Beet, 1212 18th St NW, 20036, +1 202-796-5100</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>March</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,26 +221,26 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -236,10 +257,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -274,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -326,7 +347,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -437,21 +458,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -468,7 +489,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -520,27 +541,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -568,73 +590,183 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="75.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
-  <dimension ref="A1:D1"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -642,40 +774,78 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
-  <dimension ref="A1:F3"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -715,19 +885,19 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D3" s="3">
         <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F3" s="3">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -735,16 +905,16 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
-  <dimension ref="A1:F2"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:F2"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,13 +956,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
-  <dimension ref="A1:H2"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -800,17 +970,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -851,14 +1021,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
-  <dimension ref="A1:I2"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -866,65 +1036,65 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Syndication Report and abstract methods
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aneeshc\git\DACAutomation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{B1B9883B-8408-4C7B-9A47-C46A7D0902DB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{C52699B9-2761-4AA5-AAD4-68F79B973231}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView activeTab="5" windowHeight="15840" windowWidth="29040" xWindow="20370" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
+    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
@@ -19,9 +19,10 @@
     <sheet name="Duplicate_Management" r:id="rId4" sheetId="7"/>
     <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
     <sheet name="Zoom" r:id="rId6" sheetId="2"/>
-    <sheet name="PDF" r:id="rId7" sheetId="3"/>
-    <sheet name="SA_Filters" r:id="rId8" sheetId="4"/>
-    <sheet name="SA_Advanced_Filters" r:id="rId9" sheetId="5"/>
+    <sheet name="Syndication" r:id="rId7" sheetId="10"/>
+    <sheet name="PDF" r:id="rId8" sheetId="3"/>
+    <sheet name="SA_Filters" r:id="rId9" sheetId="4"/>
+    <sheet name="SA_Advanced_Filters" r:id="rId10" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="52">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -165,6 +166,30 @@
   </si>
   <si>
     <t>March</t>
+  </si>
+  <si>
+    <t>Location Number</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>TomTom</t>
+  </si>
+  <si>
+    <t>HERE</t>
+  </si>
+  <si>
+    <t>Zomato</t>
+  </si>
+  <si>
+    <t>9990038413</t>
+  </si>
+  <si>
+    <t>'9990038413</t>
   </si>
 </sst>
 </file>
@@ -551,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,16 +618,89 @@
         <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -839,7 +937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -910,6 +1008,65 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -960,7 +1117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1024,77 +1181,4 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Syndication Status DTC Verification code in page class and test class
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{C52699B9-2761-4AA5-AAD4-68F79B973231}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D19264-6A9A-409F-9120-B58A8C86ACB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="7" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
-    <sheet name="Display_Review" r:id="rId2" sheetId="9"/>
-    <sheet name="Bing" r:id="rId3" sheetId="8"/>
-    <sheet name="Duplicate_Management" r:id="rId4" sheetId="7"/>
-    <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
-    <sheet name="Zoom" r:id="rId6" sheetId="2"/>
-    <sheet name="Syndication" r:id="rId7" sheetId="10"/>
-    <sheet name="PDF" r:id="rId8" sheetId="3"/>
-    <sheet name="SA_Filters" r:id="rId9" sheetId="4"/>
-    <sheet name="SA_Advanced_Filters" r:id="rId10" sheetId="5"/>
+    <sheet name="TPSEE" sheetId="1" r:id="rId1"/>
+    <sheet name="Display_Review" sheetId="9" r:id="rId2"/>
+    <sheet name="Bing" sheetId="8" r:id="rId3"/>
+    <sheet name="Duplicate_Management" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="Zoom" sheetId="2" r:id="rId6"/>
+    <sheet name="Syndication" sheetId="10" r:id="rId7"/>
+    <sheet name="Syndication DTCManualApi" sheetId="11" r:id="rId8"/>
+    <sheet name="PDF" sheetId="3" r:id="rId9"/>
+    <sheet name="SA_Filters" sheetId="4" r:id="rId10"/>
+    <sheet name="SA_Advanced_Filters" sheetId="5" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="59">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -190,13 +191,33 @@
   </si>
   <si>
     <t>'9990038413</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Bing</t>
+  </si>
+  <si>
+    <t>Factual</t>
+  </si>
+  <si>
+    <t>Foursquare</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,26 +267,26 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -282,10 +303,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -320,7 +341,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -372,7 +393,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -483,21 +504,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -514,7 +535,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -566,28 +587,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -631,14 +652,80 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -646,14 +733,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -704,14 +791,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
@@ -760,13 +847,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F2"/>
@@ -815,13 +902,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -829,9 +916,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="75.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="75.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -857,14 +944,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -872,8 +959,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="4" max="4" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -928,14 +1015,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
@@ -943,7 +1030,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1003,72 +1090,217 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
       <c r="B1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>49</v>
       </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
@@ -1113,72 +1345,6 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row customFormat="1" r="1" s="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code for Syndication status page class and test classes for different scenarios
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D19264-6A9A-409F-9120-B58A8C86ACB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{FE982633-6E51-4641-8449-FBFA3F4D4DD5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="7" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}"/>
+    <workbookView activeTab="7" firstSheet="2" windowHeight="7875" windowWidth="7545" xWindow="2160" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="2160"/>
   </bookViews>
   <sheets>
-    <sheet name="TPSEE" sheetId="1" r:id="rId1"/>
-    <sheet name="Display_Review" sheetId="9" r:id="rId2"/>
-    <sheet name="Bing" sheetId="8" r:id="rId3"/>
-    <sheet name="Duplicate_Management" sheetId="7" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
-    <sheet name="Zoom" sheetId="2" r:id="rId6"/>
-    <sheet name="Syndication" sheetId="10" r:id="rId7"/>
-    <sheet name="Syndication DTCManualApi" sheetId="11" r:id="rId8"/>
-    <sheet name="PDF" sheetId="3" r:id="rId9"/>
-    <sheet name="SA_Filters" sheetId="4" r:id="rId10"/>
-    <sheet name="SA_Advanced_Filters" sheetId="5" r:id="rId11"/>
+    <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
+    <sheet name="Display_Review" r:id="rId2" sheetId="9"/>
+    <sheet name="Bing" r:id="rId3" sheetId="8"/>
+    <sheet name="Duplicate_Management" r:id="rId4" sheetId="7"/>
+    <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
+    <sheet name="Zoom" r:id="rId6" sheetId="2"/>
+    <sheet name="Syndication" r:id="rId7" sheetId="10"/>
+    <sheet name="Syndication DTCManualApi" r:id="rId8" sheetId="11"/>
+    <sheet name="PDF" r:id="rId9" sheetId="3"/>
+    <sheet name="SA_Filters" r:id="rId10" sheetId="4"/>
+    <sheet name="SA_Advanced_Filters" r:id="rId11" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="59">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -218,6 +218,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -267,26 +268,26 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -303,10 +304,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -341,7 +342,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -393,7 +394,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -504,21 +505,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -535,7 +536,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -587,15 +588,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -603,12 +604,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -652,14 +653,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -667,17 +668,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -718,14 +719,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -733,14 +734,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -791,14 +792,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
@@ -847,13 +848,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F2"/>
@@ -902,13 +903,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -916,9 +917,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="75.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="75.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -944,14 +945,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -959,8 +960,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1015,14 +1016,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
@@ -1030,7 +1031,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1090,13 +1091,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C5"/>
@@ -1104,9 +1105,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1165,21 +1166,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1193,56 +1196,56 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row customFormat="1" r="3" s="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>53</v>
@@ -1253,10 +1256,10 @@
         <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1264,7 +1267,7 @@
         <v>51</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>58</v>
@@ -1275,32 +1278,21 @@
         <v>51</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
@@ -1345,6 +1337,6 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the issues found for verifying the status
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{FE982633-6E51-4641-8449-FBFA3F4D4DD5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{677A3889-7F4B-4DC2-BB4F-F5A60A9AFA07}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView activeTab="7" firstSheet="2" windowHeight="7875" windowWidth="7545" xWindow="2160" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="2160"/>
+    <workbookView activeTab="9" firstSheet="5" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
@@ -20,10 +20,12 @@
     <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
     <sheet name="Zoom" r:id="rId6" sheetId="2"/>
     <sheet name="Syndication" r:id="rId7" sheetId="10"/>
-    <sheet name="Syndication DTCManualApi" r:id="rId8" sheetId="11"/>
-    <sheet name="PDF" r:id="rId9" sheetId="3"/>
-    <sheet name="SA_Filters" r:id="rId10" sheetId="4"/>
-    <sheet name="SA_Advanced_Filters" r:id="rId11" sheetId="5"/>
+    <sheet name="Syndication DTCManual" r:id="rId8" sheetId="11"/>
+    <sheet name="Syndication DTCAPI" r:id="rId9" sheetId="13"/>
+    <sheet name="SyndicationLPAD" r:id="rId10" sheetId="12"/>
+    <sheet name="PDF" r:id="rId11" sheetId="3"/>
+    <sheet name="SA_Filters" r:id="rId12" sheetId="4"/>
+    <sheet name="SA_Advanced_Filters" r:id="rId13" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="67">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -190,28 +192,52 @@
     <t>9990038413</t>
   </si>
   <si>
-    <t>'9990038413</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
     <t>Submitted</t>
   </si>
   <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>Bing</t>
-  </si>
-  <si>
-    <t>Factual</t>
-  </si>
-  <si>
-    <t>Foursquare</t>
-  </si>
-  <si>
-    <t>In Progress</t>
+    <t>Apple,Bing,Facebook,Factual,Foursquare,Google,HERE,TomTom</t>
+  </si>
+  <si>
+    <t>In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress</t>
+  </si>
+  <si>
+    <t>Deleted</t>
+  </si>
+  <si>
+    <t>Merged</t>
+  </si>
+  <si>
+    <t>Suppressed</t>
+  </si>
+  <si>
+    <t>Not a duplicate</t>
+  </si>
+  <si>
+    <t>Unable to process</t>
+  </si>
+  <si>
+    <t>9000223167</t>
+  </si>
+  <si>
+    <t>In Progress,In Progress,In Progress,In Progress,In Progress,Submitted,In Progress,Submitted</t>
+  </si>
+  <si>
+    <t>Pot_Dup_Location Number</t>
+  </si>
+  <si>
+    <t>Pot_Dup_Ph Number</t>
+  </si>
+  <si>
+    <t>+1 917-388-9488</t>
+  </si>
+  <si>
+    <t>9000223168</t>
+  </si>
+  <si>
+    <t>50051000516</t>
   </si>
 </sst>
 </file>
@@ -219,7 +245,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +275,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF393939"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -271,7 +303,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -281,6 +313,7 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -659,6 +692,100 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="59.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="83.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -724,7 +851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -909,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,9 +1047,12 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="75.7109375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>31</v>
       </c>
@@ -932,8 +1062,20 @@
       <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -942,6 +1084,50 @@
       </c>
       <c r="C2" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1100,14 +1286,14 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1118,7 +1304,7 @@
         <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1129,40 +1315,31 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
       <c r="B3" t="s">
         <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
       <c r="B4" t="s">
         <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>51</v>
-      </c>
       <c r="B5" t="s">
         <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1172,17 +1349,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="59.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="83.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1193,7 +1371,7 @@
         <v>45</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1201,87 +1379,10 @@
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row customFormat="1" r="3" s="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row customFormat="1" r="4" s="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row customFormat="1" r="5" s="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row customFormat="1" r="6" s="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1291,52 +1392,13 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Duplicate Management, CF, LPAD, DTC  and Syndication status page and test classes
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,35 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08DFCEF-08E5-4BCE-B033-DA0742820B24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{3D9C92F3-E080-47A3-BEC2-314AC62B2035}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}"/>
+    <workbookView activeTab="3" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="TPSEE" sheetId="1" r:id="rId1"/>
-    <sheet name="Display_Review" sheetId="9" r:id="rId2"/>
-    <sheet name="Bing" sheetId="8" r:id="rId3"/>
-    <sheet name="Duplicate_Management" sheetId="7" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
-    <sheet name="Zoom" sheetId="2" r:id="rId6"/>
-    <sheet name="Syndication" sheetId="10" r:id="rId7"/>
-    <sheet name="Syndication DTCManual" sheetId="11" r:id="rId8"/>
-    <sheet name="Syndication DTCAPI" sheetId="13" r:id="rId9"/>
-    <sheet name="SyndicationLPAD" sheetId="12" r:id="rId10"/>
-    <sheet name="PDF" sheetId="3" r:id="rId11"/>
-    <sheet name="SA_Filters" sheetId="4" r:id="rId12"/>
-    <sheet name="SA_Advanced_Filters" sheetId="5" r:id="rId13"/>
+    <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
+    <sheet name="Display_Review" r:id="rId2" sheetId="9"/>
+    <sheet name="Bing" r:id="rId3" sheetId="8"/>
+    <sheet name="Duplicate_Management" r:id="rId4" sheetId="7"/>
+    <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
+    <sheet name="Zoom" r:id="rId6" sheetId="2"/>
+    <sheet name="Syndication" r:id="rId7" sheetId="10"/>
+    <sheet name="Syndication DTCManual" r:id="rId8" sheetId="11"/>
+    <sheet name="Syndication DTCAPI" r:id="rId9" sheetId="13"/>
+    <sheet name="SyndicationLPAD" r:id="rId10" sheetId="12"/>
+    <sheet name="PDF" r:id="rId11" sheetId="3"/>
+    <sheet name="SA_Filters" r:id="rId12" sheetId="4"/>
+    <sheet name="SA_Advanced_Filters" r:id="rId13" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="70">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>https://www.google.com/maps/place/?q=place_id:ChIJLdD4Ikv1xokRXCXMOatucy4</t>
-  </si>
-  <si>
-    <t>Action Value</t>
   </si>
   <si>
     <t>except GMB , Face book , Bing</t>
@@ -256,6 +253,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -311,27 +309,27 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -348,10 +346,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -386,7 +384,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -438,7 +436,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -549,21 +547,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -580,7 +578,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -632,15 +630,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -648,12 +646,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -681,7 +679,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -697,14 +695,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -712,53 +710,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="107" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="107.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>67</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
@@ -803,13 +801,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -817,17 +815,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -868,14 +866,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -883,14 +881,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -941,14 +939,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
@@ -981,7 +979,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -997,13 +995,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F2"/>
@@ -1036,7 +1034,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -1052,26 +1050,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
-  <dimension ref="A1:G1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="75.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="75.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1082,87 +1080,81 @@
         <v>32</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>60</v>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>60</v>
+      <c r="D7" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>60</v>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -1170,14 +1162,14 @@
       <c r="G1048576" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -1185,8 +1177,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1203,7 +1195,7 @@
         <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,30 +1217,30 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>39</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
@@ -1256,7 +1248,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1296,7 +1288,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3">
         <v>2020</v>
@@ -1305,7 +1297,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" s="3">
         <v>2020</v>
@@ -1316,13 +1308,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -1330,120 +1322,120 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="102.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="102.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1451,34 +1443,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
         <v>64</v>
       </c>
-      <c r="C2" t="s">
-        <v>65</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved Null pointer exception of GR,GMB and Bing
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,35 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416AD554-ABCF-42C3-BBC5-3E54BAF11694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{3372FBFC-C267-4281-9D52-C2E2384E7840}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}"/>
+    <workbookView activeTab="5" firstSheet="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="TPSEE" sheetId="1" r:id="rId1"/>
-    <sheet name="Display_Review" sheetId="9" r:id="rId2"/>
-    <sheet name="Bing" sheetId="8" r:id="rId3"/>
-    <sheet name="Duplicate_Management" sheetId="7" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
-    <sheet name="Zoom" sheetId="2" r:id="rId6"/>
-    <sheet name="Syndication" sheetId="10" r:id="rId7"/>
-    <sheet name="Syndication DTCManual" sheetId="11" r:id="rId8"/>
-    <sheet name="Syndication DTCAPI" sheetId="13" r:id="rId9"/>
-    <sheet name="SyndicationLPAD" sheetId="12" r:id="rId10"/>
-    <sheet name="PDF" sheetId="3" r:id="rId11"/>
-    <sheet name="SA_Filters" sheetId="4" r:id="rId12"/>
-    <sheet name="SA_Advanced_Filters" sheetId="5" r:id="rId13"/>
+    <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
+    <sheet name="Display_Review" r:id="rId2" sheetId="9"/>
+    <sheet name="Bing" r:id="rId3" sheetId="8"/>
+    <sheet name="Duplicate_Management" r:id="rId4" sheetId="7"/>
+    <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
+    <sheet name="Zoom" r:id="rId6" sheetId="2"/>
+    <sheet name="Syndication" r:id="rId7" sheetId="10"/>
+    <sheet name="Syndication DTCManual" r:id="rId8" sheetId="11"/>
+    <sheet name="Syndication DTCAPI" r:id="rId9" sheetId="13"/>
+    <sheet name="SyndicationLPAD" r:id="rId10" sheetId="12"/>
+    <sheet name="PDF" r:id="rId11" sheetId="3"/>
+    <sheet name="SA_Filters" r:id="rId12" sheetId="4"/>
+    <sheet name="SA_Advanced_Filters" r:id="rId13" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -238,6 +238,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -297,28 +298,28 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -335,10 +336,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -373,7 +374,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -425,7 +426,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -536,21 +537,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -567,7 +568,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -619,15 +620,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -635,12 +636,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -684,14 +685,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -699,9 +700,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="107" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="107.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -727,14 +728,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
@@ -743,16 +744,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -779,13 +780,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -793,17 +794,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row customFormat="1" r="1" s="4" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -844,14 +845,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -859,14 +860,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -917,14 +918,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
@@ -973,13 +974,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F2"/>
@@ -1028,26 +1029,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
-  <dimension ref="A1:G1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="75.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="75.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1067,7 +1068,7 @@
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1141,16 +1142,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{F1DC5D16-654A-4D10-A0DA-C3EC9A9CD3AC}"/>
+    <hyperlink r:id="rId1" ref="B2" xr:uid="{F1DC5D16-654A-4D10-A0DA-C3EC9A9CD3AC}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -1158,8 +1159,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1214,35 +1215,35 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1289,13 +1290,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1303,9 +1304,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1355,12 +1356,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1369,10 +1370,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="102.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="102.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1386,7 +1387,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1">
+    <row customFormat="1" r="2" s="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>62</v>
       </c>
@@ -1398,14 +1399,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1413,9 +1414,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1441,6 +1442,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated account/Filters and fixed GMB issues
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{3372FBFC-C267-4281-9D52-C2E2384E7840}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{77E62FEA-76B9-450D-953C-027C05D60812}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView activeTab="5" firstSheet="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
+    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
@@ -18,14 +18,15 @@
     <sheet name="Bing" r:id="rId3" sheetId="8"/>
     <sheet name="Duplicate_Management" r:id="rId4" sheetId="7"/>
     <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
-    <sheet name="Zoom" r:id="rId6" sheetId="2"/>
-    <sheet name="Syndication" r:id="rId7" sheetId="10"/>
-    <sheet name="Syndication DTCManual" r:id="rId8" sheetId="11"/>
-    <sheet name="Syndication DTCAPI" r:id="rId9" sheetId="13"/>
-    <sheet name="SyndicationLPAD" r:id="rId10" sheetId="12"/>
-    <sheet name="PDF" r:id="rId11" sheetId="3"/>
-    <sheet name="SA_Filters" r:id="rId12" sheetId="4"/>
-    <sheet name="SA_Advanced_Filters" r:id="rId13" sheetId="5"/>
+    <sheet name="BingZoom" r:id="rId6" sheetId="14"/>
+    <sheet name="Zoom" r:id="rId7" sheetId="2"/>
+    <sheet name="Syndication" r:id="rId8" sheetId="10"/>
+    <sheet name="Syndication DTCManual" r:id="rId9" sheetId="11"/>
+    <sheet name="Syndication DTCAPI" r:id="rId10" sheetId="13"/>
+    <sheet name="SyndicationLPAD" r:id="rId11" sheetId="12"/>
+    <sheet name="PDF" r:id="rId12" sheetId="3"/>
+    <sheet name="SA_Filters" r:id="rId13" sheetId="4"/>
+    <sheet name="SA_Advanced_Filters" r:id="rId14" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="69">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -232,6 +233,18 @@
   </si>
   <si>
     <t>+966 9200 00001</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Chicago</t>
   </si>
 </sst>
 </file>
@@ -630,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -672,13 +685,13 @@
         <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>8</v>
@@ -691,6 +704,48 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -733,7 +788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -784,7 +839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -850,7 +905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -1221,11 +1276,66 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC4A950-02FB-4771-9093-D3B7699EE31D}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D2" s="3">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1294,7 +1404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -1360,7 +1470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1402,46 +1512,4 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Duplicate Management related queries
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{AD7CAC1E-C7EF-4A5C-AD5C-23C8417AB2BA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{F417D318-26AF-453A-885A-EA8886DB05E5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
+    <workbookView activeTab="3" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
@@ -28,17 +28,25 @@
     <sheet name="SA_Filters" r:id="rId13" sheetId="4"/>
     <sheet name="SA_Advanced_Filters" r:id="rId14" sheetId="5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -232,13 +240,52 @@
     <t>In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress</t>
   </si>
   <si>
-    <t>+966 9200 00001</t>
-  </si>
-  <si>
     <t>IL</t>
   </si>
   <si>
     <t>Chicago</t>
+  </si>
+  <si>
+    <t>Not a duplicate</t>
+  </si>
+  <si>
+    <t>Unable to process</t>
+  </si>
+  <si>
+    <t>DTC_Status</t>
+  </si>
+  <si>
+    <t>External Notes</t>
+  </si>
+  <si>
+    <t>Internal Notes</t>
+  </si>
+  <si>
+    <t>Testing 123</t>
+  </si>
+  <si>
+    <t>Testing 124</t>
+  </si>
+  <si>
+    <t>Testing 125</t>
+  </si>
+  <si>
+    <t>Testing 126</t>
+  </si>
+  <si>
+    <t>Testing 127</t>
+  </si>
+  <si>
+    <t>Testing 128</t>
+  </si>
+  <si>
+    <t>Testing 129</t>
+  </si>
+  <si>
+    <t>+1 610-488-2411</t>
+  </si>
+  <si>
+    <t>9000223167</t>
   </si>
 </sst>
 </file>
@@ -637,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -682,10 +729,10 @@
         <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>8</v>
@@ -1086,16 +1133,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="75.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
     <col min="6" max="7" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
   </cols>
@@ -1113,12 +1159,19 @@
       <c r="D1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>33</v>
@@ -1127,64 +1180,119 @@
         <v>50</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="C4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="C5" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="C6" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="C7" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="C8" t="s">
         <v>48</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="1048576" spans="7:7">
       <c r="G1048576" s="2"/>

</xml_diff>

<commit_message>
Updated for staging regression
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,36 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{F417D318-26AF-453A-885A-EA8886DB05E5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD0B72B-2CBE-45F9-817B-4078D0538635}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
-    <sheet name="Display_Review" r:id="rId2" sheetId="9"/>
-    <sheet name="Bing" r:id="rId3" sheetId="8"/>
-    <sheet name="Duplicate_Management" r:id="rId4" sheetId="7"/>
-    <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
-    <sheet name="BingZoom" r:id="rId6" sheetId="14"/>
-    <sheet name="Zoom" r:id="rId7" sheetId="2"/>
-    <sheet name="Syndication" r:id="rId8" sheetId="10"/>
-    <sheet name="Syndication DTCManual" r:id="rId9" sheetId="11"/>
-    <sheet name="Syndication DTCAPI" r:id="rId10" sheetId="13"/>
-    <sheet name="SyndicationLPAD" r:id="rId11" sheetId="12"/>
-    <sheet name="PDF" r:id="rId12" sheetId="3"/>
-    <sheet name="SA_Filters" r:id="rId13" sheetId="4"/>
-    <sheet name="SA_Advanced_Filters" r:id="rId14" sheetId="5"/>
+    <sheet name="TPSEE" sheetId="1" r:id="rId1"/>
+    <sheet name="Display_Review" sheetId="9" r:id="rId2"/>
+    <sheet name="Bing" sheetId="8" r:id="rId3"/>
+    <sheet name="Duplicate_Management" sheetId="7" r:id="rId4"/>
+    <sheet name="Results" sheetId="15" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="BingZoom" sheetId="14" r:id="rId7"/>
+    <sheet name="Zoom" sheetId="2" r:id="rId8"/>
+    <sheet name="Syndication" sheetId="10" r:id="rId9"/>
+    <sheet name="Syndication DTCManual" sheetId="11" r:id="rId10"/>
+    <sheet name="Syndication DTCAPI" sheetId="13" r:id="rId11"/>
+    <sheet name="SyndicationLPAD" sheetId="12" r:id="rId12"/>
+    <sheet name="PDF" sheetId="3" r:id="rId13"/>
+    <sheet name="SA_Filters" sheetId="4" r:id="rId14"/>
+    <sheet name="SA_Advanced_Filters" sheetId="5" r:id="rId15"/>
+    <sheet name="SA_Zoom" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="88">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -240,12 +242,6 @@
     <t>In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress,In Progress</t>
   </si>
   <si>
-    <t>IL</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
     <t>Not a duplicate</t>
   </si>
   <si>
@@ -282,17 +278,46 @@
     <t>Testing 129</t>
   </si>
   <si>
-    <t>+1 610-488-2411</t>
-  </si>
-  <si>
-    <t>9000223167</t>
+    <t>Resultpage</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>+1 914-202-2822</t>
+  </si>
+  <si>
+    <t>9000223153</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>26 E 40th St</t>
+  </si>
+  <si>
+    <t>August</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -352,28 +377,28 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -390,10 +415,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -428,7 +453,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -480,7 +505,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -591,21 +616,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -622,7 +647,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -674,28 +699,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F2" sqref="D2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -729,23 +754,23 @@
         <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -754,9 +779,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="102.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -767,6 +793,49 @@
         <v>41</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -782,13 +851,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -796,9 +865,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="107.0" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="107" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -824,14 +893,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
-  <dimension ref="A1:G2"/>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
@@ -876,13 +945,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
-  <dimension ref="A1:G2"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -890,17 +959,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="4" spans="1:6">
+    <row r="1" spans="1:6" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -941,14 +1010,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
-  <dimension ref="A1:J2"/>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -956,14 +1025,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1014,14 +1083,85 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3EA4CE-EDA7-4242-A743-BE83DBFF6070}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D3" s="3">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
@@ -1070,19 +1210,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="D2" sqref="D2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
@@ -1111,39 +1254,40 @@
       <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>85</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
-  <dimension ref="A1:H1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="75.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="6" max="7" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="75.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1160,18 +1304,18 @@
         <v>40</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>33</v>
@@ -1180,16 +1324,16 @@
         <v>50</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1197,16 +1341,16 @@
         <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1214,16 +1358,16 @@
         <v>49</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1231,16 +1375,16 @@
         <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1248,16 +1392,16 @@
         <v>52</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1265,16 +1409,16 @@
         <v>53</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1282,16 +1426,16 @@
         <v>48</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="1048576" spans="7:7">
@@ -1299,16 +1443,58 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2" xr:uid="{F1DC5D16-654A-4D10-A0DA-C3EC9A9CD3AC}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F1DC5D16-654A-4D10-A0DA-C3EC9A9CD3AC}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF31050-A1CE-4806-A18B-82FAF036D110}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -1316,8 +1502,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="4" max="4" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1372,17 +1558,17 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC4A950-02FB-4771-9093-D3B7699EE31D}">
-  <dimension ref="A1:G3"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC4A950-02FB-4771-9093-D3B7699EE31D}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1424,19 +1610,19 @@
         <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C3" s="3">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D3" s="3">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="F3" s="3">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -1444,21 +1630,21 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
-  <dimension ref="A1:G3"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1498,7 +1684,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C3" s="3">
         <v>2020</v>
@@ -1507,7 +1693,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="F3" s="3">
         <v>2020</v>
@@ -1518,13 +1704,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
-  <dimension ref="A1:D5"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1532,9 +1718,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1584,50 +1770,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="102.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Code for score comparison of graph and overall
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{5509D916-D5AC-49EC-9E50-A82741F08A76}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{95B69A22-587E-4C41-8487-1559DC035A07}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
     <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="87">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -303,6 +303,12 @@
   </si>
   <si>
     <t>9000223160</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>101 Maiden Ln</t>
   </si>
 </sst>
 </file>
@@ -341,13 +347,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
-      <name val="Calibri "/>
+      <sz val="10"/>
+      <color rgb="FF393939"/>
+      <name val="Open Sans"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF393939"/>
+      <color rgb="FF000000"/>
       <name val="Open Sans"/>
     </font>
   </fonts>
@@ -372,7 +378,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -380,7 +386,15 @@
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -702,7 +716,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -742,16 +756,16 @@
       <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -901,16 +915,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1091,16 +1105,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1211,43 +1225,48 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="7" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="7" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="7" width="8.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" style="7" width="9.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="7" width="47.28515625" collapsed="true"/>
+    <col min="7" max="16384" style="7" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -1255,7 +1274,7 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1306,7 +1325,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>83</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1486,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1549,6 +1568,20 @@
         <v>38</v>
       </c>
     </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
@@ -1560,22 +1593,22 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1605,7 +1638,7 @@
         <v>82</v>
       </c>
       <c r="C3" s="3">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D3" s="3">
         <v>10</v>
@@ -1614,7 +1647,7 @@
         <v>81</v>
       </c>
       <c r="F3" s="3">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
   </sheetData>
@@ -1640,16 +1673,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Completed Global filter and keyword search filter  functionalities for All Locations tab in Manage Pages page. Done Exporting data and comparing data between UI and excel
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohitm\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{C7C9D68B-5280-4E5F-8A91-B69F55881021}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{C645E2BF-B3BB-4847-833A-577FAD07BC67}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
+    <workbookView activeTab="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
+    <sheet name="Configuration" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -67,6 +68,21 @@
   </si>
   <si>
     <t>US</t>
+  </si>
+  <si>
+    <t>Country_A</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>AUH</t>
+  </si>
+  <si>
+    <t>Abu Dhabi</t>
+  </si>
+  <si>
+    <t>TestLocation5, Theyab Bin Eissa St, +971600522252</t>
   </si>
 </sst>
 </file>
@@ -428,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,4 +502,65 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7936F0-11C6-4C74-931B-7A6CA8535798}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Done Keyword search and global filter combinations for Assigned Locations
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohitm\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{C645E2BF-B3BB-4847-833A-577FAD07BC67}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{2EEC1815-DBCE-44AC-BBA8-1CA0A8ABF7CA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
     <workbookView activeTab="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
@@ -73,16 +73,16 @@
     <t>Country_A</t>
   </si>
   <si>
-    <t>AE</t>
-  </si>
-  <si>
-    <t>AUH</t>
-  </si>
-  <si>
-    <t>Abu Dhabi</t>
-  </si>
-  <si>
-    <t>TestLocation5, Theyab Bin Eissa St, +971600522252</t>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Marvel pro, Finch Ave W, M3J 3H7, +14166041496</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated scripts for TSEE Reports
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{95B69A22-587E-4C41-8487-1559DC035A07}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{13968CDE-1DB9-4084-B35B-6654E33F92B0}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
     <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="94">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -293,22 +293,43 @@
     <t>100</t>
   </si>
   <si>
-    <t>July</t>
+    <t>+1 917-338-7111</t>
+  </si>
+  <si>
+    <t>9000223160</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>101 Maiden Ln</t>
+  </si>
+  <si>
+    <t>Beta Filter</t>
+  </si>
+  <si>
+    <t>Staging Date Filter - Client Level ,User</t>
+  </si>
+  <si>
+    <t>Staging Filter - Client Level User</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>26 E 40th St</t>
   </si>
   <si>
     <t>June</t>
   </si>
   <si>
-    <t>+1 917-338-7111</t>
-  </si>
-  <si>
-    <t>9000223160</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>101 Maiden Ln</t>
+    <t xml:space="preserve">Staging Filter - Location Level User </t>
+  </si>
+  <si>
+    <t>148 Madison Ave</t>
+  </si>
+  <si>
+    <t>Staging Date Filter - Location Level</t>
   </si>
 </sst>
 </file>
@@ -378,7 +399,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -395,6 +416,7 @@
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -716,7 +738,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -756,16 +778,16 @@
       <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -915,16 +937,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1105,16 +1127,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1266,7 +1288,7 @@
         <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -1274,7 +1296,7 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1326,7 +1348,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>33</v>
@@ -1335,7 +1357,7 @@
         <v>50</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>50</v>
@@ -1352,7 +1374,7 @@
         <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>51</v>
@@ -1369,7 +1391,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>49</v>
@@ -1386,7 +1408,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>54</v>
@@ -1403,7 +1425,7 @@
         <v>52</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>64</v>
@@ -1420,7 +1442,7 @@
         <v>53</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>65</v>
@@ -1437,7 +1459,7 @@
         <v>48</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>48</v>
@@ -1505,14 +1527,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D18" sqref="B18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
@@ -1568,18 +1591,87 @@
         <v>38</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="10">
+        <v>43991</v>
+      </c>
+      <c r="B14" s="10">
+        <v>44063</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="10">
+        <v>44013</v>
+      </c>
+      <c r="B21" s="10">
+        <v>44063</v>
       </c>
     </row>
   </sheetData>
@@ -1593,22 +1685,22 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1632,22 +1724,22 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C3" s="3">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D3" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F3" s="3">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -1664,7 +1756,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1673,16 +1765,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1706,19 +1798,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C3" s="3">
         <v>2020</v>
       </c>
       <c r="D3" s="3">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F3" s="3">
         <v>2020</v>

</xml_diff>

<commit_message>
Updated Reviews Feed and Reviews Insights
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{13968CDE-1DB9-4084-B35B-6654E33F92B0}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{D615A604-472F-4D42-B05A-F3D0AB8F834A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
     <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="99">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -320,9 +320,6 @@
     <t>26 E 40th St</t>
   </si>
   <si>
-    <t>June</t>
-  </si>
-  <si>
     <t xml:space="preserve">Staging Filter - Location Level User </t>
   </si>
   <si>
@@ -330,6 +327,24 @@
   </si>
   <si>
     <t>Staging Date Filter - Location Level</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>125 Westchester Ave</t>
+  </si>
+  <si>
+    <t>White Plains</t>
+  </si>
+  <si>
+    <t>Fields Good Chicken</t>
   </si>
 </sst>
 </file>
@@ -399,7 +414,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -408,9 +423,6 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
@@ -738,7 +750,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -775,14 +787,14 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -937,16 +949,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1127,16 +1139,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1247,7 +1259,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1284,14 +1296,14 @@
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>39</v>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -1527,15 +1539,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="B18:D18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
@@ -1606,7 +1619,7 @@
       <c r="C7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1617,15 +1630,18 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>83</v>
       </c>
       <c r="C10" t="s">
         <v>83</v>
       </c>
       <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1635,19 +1651,19 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <v>43991</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>44063</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1658,20 +1674,37 @@
         <v>83</v>
       </c>
       <c r="D18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="10">
+    <row r="21" spans="1:5">
+      <c r="A21" s="9">
         <v>44013</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>44063</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1685,22 +1718,22 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="A3:F3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1727,16 +1760,16 @@
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C3" s="3">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D3" s="3">
         <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F3" s="3">
         <v>2020</v>
@@ -1756,7 +1789,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1765,16 +1798,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1801,13 +1834,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C3" s="3">
         <v>2020</v>
       </c>
       <c r="D3" s="3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>88</v>

</xml_diff>

<commit_message>
Updated Reviews and TSEE Reports
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{D615A604-472F-4D42-B05A-F3D0AB8F834A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
+  <xr:revisionPtr documentId="13_ncr:1_{823B31BD-C09B-44EE-BF32-BBB296E0DED1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
     <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
@@ -750,7 +750,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -797,10 +797,10 @@
         <v>83</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1541,8 +1541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added additional scenario - Verification of filter data - Order of data.
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,34 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{16E7265B-FBE1-45CB-A6FB-B7E115E2066C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
+  <xr:revisionPtr documentId="13_ncr:1_{ABF6DDBC-755E-4673-9CE4-BE8B24B74E85}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
+    <workbookView activeTab="6" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
-    <sheet name="Display_Review" r:id="rId2" sheetId="9"/>
-    <sheet name="Bing" r:id="rId3" sheetId="8"/>
-    <sheet name="Duplicate_Management" r:id="rId4" sheetId="7"/>
-    <sheet name="Results" r:id="rId5" sheetId="15"/>
-    <sheet name="Sheet1" r:id="rId6" sheetId="6"/>
-    <sheet name="BingZoom" r:id="rId7" sheetId="14"/>
-    <sheet name="Zoom" r:id="rId8" sheetId="2"/>
-    <sheet name="Syndication" r:id="rId9" sheetId="10"/>
-    <sheet name="Syndication DTCManual" r:id="rId10" sheetId="11"/>
-    <sheet name="Syndication DTCAPI" r:id="rId11" sheetId="13"/>
-    <sheet name="SyndicationLPAD" r:id="rId12" sheetId="12"/>
-    <sheet name="PDF" r:id="rId13" sheetId="3"/>
-    <sheet name="SA_Filters" r:id="rId14" sheetId="4"/>
-    <sheet name="SA_Advanced_Filters" r:id="rId15" sheetId="5"/>
-    <sheet name="SA_Zoom" r:id="rId16" sheetId="16"/>
+    <sheet name="Facebook" r:id="rId2" sheetId="20"/>
+    <sheet name="Display_Review" r:id="rId3" sheetId="9"/>
+    <sheet name="Bing" r:id="rId4" sheetId="8"/>
+    <sheet name="FilterOrder" r:id="rId5" sheetId="17"/>
+    <sheet name="FilterOrderBing" r:id="rId6" sheetId="18"/>
+    <sheet name="FilterOrderFacebook" r:id="rId7" sheetId="19"/>
+    <sheet name="Duplicate_Management" r:id="rId8" sheetId="7"/>
+    <sheet name="Results" r:id="rId9" sheetId="15"/>
+    <sheet name="Sheet1" r:id="rId10" sheetId="6"/>
+    <sheet name="BingZoom" r:id="rId11" sheetId="14"/>
+    <sheet name="Zoom" r:id="rId12" sheetId="2"/>
+    <sheet name="Syndication" r:id="rId13" sheetId="10"/>
+    <sheet name="Syndication DTCManual" r:id="rId14" sheetId="11"/>
+    <sheet name="Syndication DTCAPI" r:id="rId15" sheetId="13"/>
+    <sheet name="SyndicationLPAD" r:id="rId16" sheetId="12"/>
+    <sheet name="PDF" r:id="rId17" sheetId="3"/>
+    <sheet name="SA_Filters" r:id="rId18" sheetId="4"/>
+    <sheet name="SA_Advanced_Filters" r:id="rId19" sheetId="5"/>
+    <sheet name="SA_Zoom" r:id="rId20" sheetId="16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="103">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -342,6 +346,21 @@
   </si>
   <si>
     <t>Automation Test</t>
+  </si>
+  <si>
+    <t>All Locations</t>
+  </si>
+  <si>
+    <t>0302</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Thrissur</t>
   </si>
 </sst>
 </file>
@@ -411,7 +430,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -426,6 +445,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -746,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -796,7 +818,7 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
@@ -807,6 +829,396 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="9">
+        <v>43991</v>
+      </c>
+      <c r="B14" s="9">
+        <v>44063</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="9">
+        <v>44013</v>
+      </c>
+      <c r="B21" s="9">
+        <v>44063</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC4A950-02FB-4771-9093-D3B7699EE31D}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D3" s="3">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D3" s="3">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -850,7 +1262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -892,7 +1304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -935,7 +1347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -946,16 +1358,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -986,7 +1398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1052,7 +1464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -1125,7 +1537,62 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F635368-BB2D-4072-8E80-91DBE792F8EF}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3EA4CE-EDA7-4242-A743-BE83DBFF6070}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1136,16 +1603,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1196,7 +1663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1251,7 +1718,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1305,7 +1772,7 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1315,7 +1782,161 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0C12BF-7E83-4532-A128-E57EBFF1BF2D}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2DE816-A9A4-4743-BF9C-2DEBCA2D1E71}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row ht="26.25" r="2" spans="1:5">
+      <c r="A2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97167B2-7C0B-4E15-B189-0ACF08094BA1}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row ht="26.25" r="2" spans="1:5">
+      <c r="A2" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
   <dimension ref="A1:H1048576"/>
   <sheetViews>
@@ -1492,7 +2113,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF31050-A1CE-4806-A18B-82FAF036D110}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1532,394 +2153,4 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
-  <dimension ref="A1:F25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="B10:E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="9">
-        <v>43991</v>
-      </c>
-      <c r="B14" s="9">
-        <v>44063</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="9">
-        <v>44013</v>
-      </c>
-      <c r="B21" s="9">
-        <v>44063</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC4A950-02FB-4771-9093-D3B7699EE31D}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2020</v>
-      </c>
-      <c r="D3" s="3">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="3">
-        <v>2020</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-  </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2020</v>
-      </c>
-      <c r="D3" s="3">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="3">
-        <v>2020</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-  </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated handling filter combination for TSEE reports and single execution for all scenarios
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{ABF6DDBC-755E-4673-9CE4-BE8B24B74E85}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
+  <xr:revisionPtr documentId="13_ncr:1_{FBAF4D26-5352-4DF8-BC16-AE5CA9AEA214}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
+    <workbookView activeTab="12" firstSheet="8" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
@@ -23,16 +23,17 @@
     <sheet name="Duplicate_Management" r:id="rId8" sheetId="7"/>
     <sheet name="Results" r:id="rId9" sheetId="15"/>
     <sheet name="Sheet1" r:id="rId10" sheetId="6"/>
-    <sheet name="BingZoom" r:id="rId11" sheetId="14"/>
-    <sheet name="Zoom" r:id="rId12" sheetId="2"/>
-    <sheet name="Syndication" r:id="rId13" sheetId="10"/>
-    <sheet name="Syndication DTCManual" r:id="rId14" sheetId="11"/>
-    <sheet name="Syndication DTCAPI" r:id="rId15" sheetId="13"/>
-    <sheet name="SyndicationLPAD" r:id="rId16" sheetId="12"/>
-    <sheet name="PDF" r:id="rId17" sheetId="3"/>
-    <sheet name="SA_Filters" r:id="rId18" sheetId="4"/>
-    <sheet name="SA_Advanced_Filters" r:id="rId19" sheetId="5"/>
-    <sheet name="SA_Zoom" r:id="rId20" sheetId="16"/>
+    <sheet name="New Filters" r:id="rId11" sheetId="21"/>
+    <sheet name="BingZoom" r:id="rId12" sheetId="14"/>
+    <sheet name="Zoom" r:id="rId13" sheetId="2"/>
+    <sheet name="Syndication" r:id="rId14" sheetId="10"/>
+    <sheet name="Syndication DTCManual" r:id="rId15" sheetId="11"/>
+    <sheet name="Syndication DTCAPI" r:id="rId16" sheetId="13"/>
+    <sheet name="SyndicationLPAD" r:id="rId17" sheetId="12"/>
+    <sheet name="PDF" r:id="rId18" sheetId="3"/>
+    <sheet name="SA_Filters" r:id="rId19" sheetId="4"/>
+    <sheet name="SA_Advanced_Filters" r:id="rId20" sheetId="5"/>
+    <sheet name="SA_Zoom" r:id="rId21" sheetId="16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="115">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -318,9 +319,6 @@
     <t>Staging Filter - Client Level User</t>
   </si>
   <si>
-    <t>August</t>
-  </si>
-  <si>
     <t>26 E 40th St</t>
   </si>
   <si>
@@ -333,12 +331,6 @@
     <t>Staging Date Filter - Location Level</t>
   </si>
   <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>125 Westchester Ave</t>
-  </si>
-  <si>
     <t>White Plains</t>
   </si>
   <si>
@@ -351,16 +343,61 @@
     <t>All Locations</t>
   </si>
   <si>
-    <t>0302</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>Kerala</t>
-  </si>
-  <si>
-    <t>Thrissur</t>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>Scenario5</t>
+  </si>
+  <si>
+    <t>Scenario2</t>
+  </si>
+  <si>
+    <t>Scenario3</t>
+  </si>
+  <si>
+    <t>Scenario4</t>
+  </si>
+  <si>
+    <t>Scenario6</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>Melt Shop, 125 Westchester Ave, Westchester Mall, Savor Food Hall L4, 10601, (914) 202-2822</t>
+  </si>
+  <si>
+    <t>Automation Account - Filter Combination - Client Level</t>
+  </si>
+  <si>
+    <t>Automation Account - Date Filter - Client Level</t>
+  </si>
+  <si>
+    <t>International Account - Filter Combination - Client Level</t>
+  </si>
+  <si>
+    <t>International Account - Date Filter - Client Level</t>
+  </si>
+  <si>
+    <t>Bing and Facebook</t>
+  </si>
+  <si>
+    <t>Location Level</t>
+  </si>
+  <si>
+    <t>Automation Account - Filter Combination - Location Level</t>
+  </si>
+  <si>
+    <t>Automation Account - Date Filter - Location Level</t>
+  </si>
+  <si>
+    <t>International Account - Filter Combination - Location Level</t>
+  </si>
+  <si>
+    <t>International Account - Date Filter - Location Level</t>
   </si>
 </sst>
 </file>
@@ -368,7 +405,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +445,12 @@
       <color rgb="FF000000"/>
       <name val="Open Sans"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -430,7 +473,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -447,6 +490,9 @@
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
@@ -766,13 +812,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
@@ -782,7 +828,7 @@
     <col min="6" max="6" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -820,6 +866,106 @@
       </c>
       <c r="F2" s="8" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -832,11 +978,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
@@ -844,7 +990,7 @@
     <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -861,7 +1007,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -878,7 +1024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
@@ -895,14 +1041,14 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>27</v>
@@ -917,14 +1063,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
@@ -936,15 +1082,15 @@
         <v>83</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>43991</v>
       </c>
@@ -952,31 +1098,31 @@
         <v>44063</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>44013</v>
       </c>
@@ -984,7 +1130,7 @@
         <v>44063</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -995,10 +1141,10 @@
         <v>83</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1008,102 +1154,700 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC4A950-02FB-4771-9093-D3B7699EE31D}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73840A65-FD3F-4FC7-8FDF-F89283B3CCE3}">
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row ht="45" r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row ht="30" r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23">
+        <v>2021</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row ht="45" r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
+      <c r="B37" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D37" s="3">
+        <v>2</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" s="3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2020</v>
-      </c>
-      <c r="D3" s="3">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="3">
-        <v>2020</v>
-      </c>
+      <c r="B49" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="2">
+        <v>2021</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F49" s="2">
+        <v>2021</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC4A950-02FB-4771-9093-D3B7699EE31D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1123,24 +1867,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2020</v>
-      </c>
-      <c r="D3" s="3">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="3">
-        <v>2020</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2021</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>
@@ -1153,223 +1897,31 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="102.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="107.0" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1387,6 +1939,26 @@
       </c>
       <c r="F2" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>
@@ -1398,7 +1970,253 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="102.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="107.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1406,7 +2224,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
@@ -1418,7 +2236,7 @@
     <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="4" spans="1:6">
+    <row customFormat="1" r="1" s="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1438,7 +2256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1464,7 +2282,145 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F635368-BB2D-4072-8E80-91DBE792F8EF}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" customWidth="true" width="13.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -1472,7 +2428,7 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
@@ -1484,7 +2440,7 @@
     <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -1511,7 +2467,7 @@
       </c>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1537,62 +2493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F635368-BB2D-4072-8E80-91DBE792F8EF}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3EA4CE-EDA7-4242-A743-BE83DBFF6070}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1600,21 +2501,21 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1634,7 +2535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>19</v>
       </c>
@@ -1671,9 +2572,9 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1693,7 +2594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1720,23 +2621,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" style="7" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="7" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="7" width="9.42578125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="7" width="8.0" collapsed="true"/>
     <col min="4" max="5" bestFit="true" customWidth="true" style="7" width="9.42578125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="7" width="47.28515625" collapsed="true"/>
     <col min="7" max="16384" style="7" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1756,8 +2657,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1774,6 +2675,86 @@
       </c>
       <c r="F2" s="8" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1787,15 +2768,16 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1812,9 +2794,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row ht="15.75" r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>27</v>
@@ -1826,7 +2808,7 @@
         <v>83</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1840,15 +2822,15 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1865,9 +2847,9 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="26.25" r="2" spans="1:5">
+    <row ht="15.75" r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>27</v>
@@ -1879,7 +2861,7 @@
         <v>83</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1891,13 +2873,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97167B2-7C0B-4E15-B189-0ACF08094BA1}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1914,21 +2896,21 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="26.25" r="2" spans="1:5">
+    <row ht="15.75" r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1944,7 +2926,7 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="75.7109375" collapsed="true"/>
@@ -1953,7 +2935,7 @@
     <col min="6" max="7" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>31</v>
       </c>
@@ -1976,7 +2958,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row ht="15.75" r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>81</v>
       </c>
@@ -1999,7 +2981,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>51</v>
       </c>
@@ -2016,7 +2998,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>49</v>
       </c>
@@ -2033,7 +3015,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>54</v>
       </c>
@@ -2050,7 +3032,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>52</v>
       </c>
@@ -2067,7 +3049,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>53</v>
       </c>
@@ -2084,7 +3066,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>48</v>
       </c>
@@ -2101,7 +3083,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="1048576" spans="7:7">
+    <row r="1048576" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G1048576" s="2"/>
     </row>
   </sheetData>
@@ -2119,32 +3101,32 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
1)Updated active and inactive state of reports
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{FBAF4D26-5352-4DF8-BC16-AE5CA9AEA214}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{00CC6A2A-39E5-4AF7-9B35-CCB450073262}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="12" firstSheet="8" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
+    <workbookView activeTab="3" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="123">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -398,6 +398,30 @@
   </si>
   <si>
     <t>International Account - Date Filter - Location Level</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Staging</t>
+  </si>
+  <si>
+    <t>Test Automation</t>
+  </si>
+  <si>
+    <t>135 W 50th St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aurify Brands - Filter Combination - Client Level </t>
+  </si>
+  <si>
+    <t>Aurify Brands - Date Filter - Client Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aurify Brands - Filter Combination - Location Level </t>
+  </si>
+  <si>
+    <t>Aurify Brands - Date Filter - Location Level</t>
   </si>
 </sst>
 </file>
@@ -405,7 +429,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -451,6 +475,19 @@
       <name val="Open Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF393939"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -473,7 +510,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -494,6 +531,10 @@
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -849,7 +890,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -950,7 +991,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>94</v>
@@ -1155,20 +1196,28 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73840A65-FD3F-4FC7-8FDF-F89283B3CCE3}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:F37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1188,7 +1237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>99</v>
       </c>
@@ -1208,7 +1257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>100</v>
       </c>
@@ -1228,7 +1277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>101</v>
       </c>
@@ -1248,7 +1297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>98</v>
       </c>
@@ -1268,7 +1317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row ht="45" r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row ht="45" r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>102</v>
       </c>
@@ -1288,12 +1337,19 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -1313,15 +1369,25 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H14" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="4"/>
+      <c r="J14" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1341,7 +1407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>99</v>
       </c>
@@ -1361,7 +1427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>100</v>
       </c>
@@ -1381,7 +1447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>101</v>
       </c>
@@ -1401,7 +1467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row ht="30" r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row ht="30" r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>98</v>
       </c>
@@ -1421,7 +1487,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1429,12 +1495,19 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1454,19 +1527,22 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2" t="s">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -1486,7 +1562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>99</v>
       </c>
@@ -1506,7 +1582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>100</v>
       </c>
@@ -1526,7 +1602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>101</v>
       </c>
@@ -1546,7 +1622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
@@ -1566,7 +1642,7 @@
         <v>8</v>
       </c>
     </row>
-    <row ht="45" r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row ht="45" r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>102</v>
       </c>
@@ -1586,7 +1662,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1594,7 +1670,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1602,17 +1678,20 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>11</v>
       </c>
@@ -1632,22 +1711,25 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="4"/>
+      <c r="J40" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>6</v>
       </c>
@@ -1670,7 +1752,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>99</v>
       </c>
@@ -1678,7 +1760,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>8</v>
@@ -1693,7 +1775,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>100</v>
       </c>
@@ -1701,10 +1783,10 @@
         <v>7</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>8</v>
@@ -1716,7 +1798,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>101</v>
       </c>
@@ -1724,13 +1806,13 @@
         <v>7</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>8</v>
@@ -1739,7 +1821,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row ht="45" r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>98</v>
       </c>
@@ -1747,22 +1829,22 @@
         <v>7</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1773,7 +1855,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1784,16 +1866,18 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
@@ -1820,8 +1904,728 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row ht="15.75" r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>11</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D63" s="3">
+        <v>2</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F63" s="3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G70" s="2"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G71" s="2"/>
+    </row>
+    <row ht="15.75" r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F72" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>11</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C76" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D76" s="3">
+        <v>2</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F76" s="3">
+        <v>2021</v>
+      </c>
+      <c r="G76" s="2"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row ht="15.75" r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F85" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="3">
+        <v>18</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C89" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D89" s="3">
+        <v>2</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F89" s="3">
+        <v>2021</v>
+      </c>
+      <c r="G89" s="2"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F94" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G94" s="2"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G95" s="2"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F96" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G96" s="2"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F97" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G97" s="2"/>
+    </row>
+    <row ht="15.75" r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F98" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G98" s="2"/>
+    </row>
+    <row ht="15.75" r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="2"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="3">
+        <v>18</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C103" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D103" s="3">
+        <v>2</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F103" s="3">
+        <v>2021</v>
+      </c>
+      <c r="G103" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1836,16 +2640,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1868,22 +2672,22 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="A3" s="3">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="3">
         <v>2021</v>
       </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>2021</v>
       </c>
     </row>
@@ -1900,7 +2704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
@@ -1910,16 +2714,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1943,10 +2747,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C3" s="3">
         <v>2021</v>
@@ -1955,7 +2759,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3">
         <v>2021</v>
@@ -2176,16 +2980,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2284,10 +3088,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F635368-BB2D-4072-8E80-91DBE792F8EF}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F6"/>
+      <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2340,10 +3144,10 @@
         <v>99</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -2360,13 +3164,13 @@
         <v>100</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -2380,7 +3184,7 @@
         <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>27</v>
@@ -2389,7 +3193,7 @@
         <v>83</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>8</v>
@@ -2400,7 +3204,7 @@
         <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>27</v>
@@ -2411,8 +3215,28 @@
       <c r="E6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>88</v>
+      <c r="F6" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2504,16 +3328,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2621,10 +3445,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2682,10 +3506,10 @@
         <v>99</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -2702,13 +3526,13 @@
         <v>100</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -2722,7 +3546,7 @@
         <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>27</v>
@@ -2731,7 +3555,7 @@
         <v>83</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>8</v>
@@ -2742,7 +3566,7 @@
         <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>27</v>
@@ -2753,8 +3577,28 @@
       <c r="E6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>88</v>
+      <c r="F6" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated search filter scenarios
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,43 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{00CC6A2A-39E5-4AF7-9B35-CCB450073262}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DA76FC-9677-4651-B633-6C025050DD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
-    <sheet name="Facebook" r:id="rId2" sheetId="20"/>
-    <sheet name="Display_Review" r:id="rId3" sheetId="9"/>
-    <sheet name="Bing" r:id="rId4" sheetId="8"/>
-    <sheet name="FilterOrder" r:id="rId5" sheetId="17"/>
-    <sheet name="FilterOrderBing" r:id="rId6" sheetId="18"/>
-    <sheet name="FilterOrderFacebook" r:id="rId7" sheetId="19"/>
-    <sheet name="Duplicate_Management" r:id="rId8" sheetId="7"/>
-    <sheet name="Results" r:id="rId9" sheetId="15"/>
-    <sheet name="Sheet1" r:id="rId10" sheetId="6"/>
-    <sheet name="New Filters" r:id="rId11" sheetId="21"/>
-    <sheet name="BingZoom" r:id="rId12" sheetId="14"/>
-    <sheet name="Zoom" r:id="rId13" sheetId="2"/>
-    <sheet name="Syndication" r:id="rId14" sheetId="10"/>
-    <sheet name="Syndication DTCManual" r:id="rId15" sheetId="11"/>
-    <sheet name="Syndication DTCAPI" r:id="rId16" sheetId="13"/>
-    <sheet name="SyndicationLPAD" r:id="rId17" sheetId="12"/>
-    <sheet name="PDF" r:id="rId18" sheetId="3"/>
-    <sheet name="SA_Filters" r:id="rId19" sheetId="4"/>
-    <sheet name="SA_Advanced_Filters" r:id="rId20" sheetId="5"/>
-    <sheet name="SA_Zoom" r:id="rId21" sheetId="16"/>
+    <sheet name="TPSEE" sheetId="1" r:id="rId1"/>
+    <sheet name="Location_Page_Search" sheetId="22" r:id="rId2"/>
+    <sheet name="Facebook" sheetId="20" r:id="rId3"/>
+    <sheet name="Display_Review" sheetId="9" r:id="rId4"/>
+    <sheet name="Bing" sheetId="8" r:id="rId5"/>
+    <sheet name="FilterOrder" sheetId="17" r:id="rId6"/>
+    <sheet name="FilterOrderBing" sheetId="18" r:id="rId7"/>
+    <sheet name="FilterOrderFacebook" sheetId="19" r:id="rId8"/>
+    <sheet name="Duplicate_Management" sheetId="7" r:id="rId9"/>
+    <sheet name="Results" sheetId="15" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId11"/>
+    <sheet name="New Filters" sheetId="21" r:id="rId12"/>
+    <sheet name="BingZoom" sheetId="14" r:id="rId13"/>
+    <sheet name="Zoom" sheetId="2" r:id="rId14"/>
+    <sheet name="Syndication" sheetId="10" r:id="rId15"/>
+    <sheet name="Syndication DTCManual" sheetId="11" r:id="rId16"/>
+    <sheet name="Syndication DTCAPI" sheetId="13" r:id="rId17"/>
+    <sheet name="SyndicationLPAD" sheetId="12" r:id="rId18"/>
+    <sheet name="PDF" sheetId="3" r:id="rId19"/>
+    <sheet name="SA_Filters" sheetId="4" r:id="rId20"/>
+    <sheet name="SA_Advanced_Filters" sheetId="5" r:id="rId21"/>
+    <sheet name="SA_Zoom" sheetId="16" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="134">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -422,13 +423,45 @@
   </si>
   <si>
     <t>Aurify Brands - Date Filter - Location Level</t>
+  </si>
+  <si>
+    <t>Search By Location</t>
+  </si>
+  <si>
+    <t>Search By Name</t>
+  </si>
+  <si>
+    <t>Search By Address</t>
+  </si>
+  <si>
+    <t>Search By City</t>
+  </si>
+  <si>
+    <t>Search By State</t>
+  </si>
+  <si>
+    <t>Search By Postal Code</t>
+  </si>
+  <si>
+    <t>Search By Phone</t>
+  </si>
+  <si>
+    <t>9000230163</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>55425</t>
+  </si>
+  <si>
+    <t>+1 703-310-6711</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -507,44 +540,45 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -561,10 +595,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -599,7 +633,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -651,7 +685,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -762,21 +796,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -793,7 +827,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -845,15 +879,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F7"/>
@@ -861,12 +895,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1010,14 +1044,56 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
-  <dimension ref="A1:F25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF31050-A1CE-4806-A18B-82FAF036D110}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A25" sqref="A25:E25"/>
@@ -1025,10 +1101,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1189,14 +1265,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73840A65-FD3F-4FC7-8FDF-F89283B3CCE3}">
-  <dimension ref="A1:K103"/>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73840A65-FD3F-4FC7-8FDF-F89283B3CCE3}">
+  <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F7"/>
@@ -1317,7 +1393,7 @@
         <v>8</v>
       </c>
     </row>
-    <row ht="45" r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>102</v>
       </c>
@@ -1467,7 +1543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row ht="30" r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>98</v>
       </c>
@@ -1642,7 +1718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row ht="45" r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>102</v>
       </c>
@@ -1821,7 +1897,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row ht="45" r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>98</v>
       </c>
@@ -2017,7 +2093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row ht="15.75" r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>102</v>
       </c>
@@ -2204,7 +2280,7 @@
       </c>
       <c r="G71" s="2"/>
     </row>
-    <row ht="15.75" r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>102</v>
       </c>
@@ -2390,7 +2466,7 @@
         <v>8</v>
       </c>
     </row>
-    <row ht="15.75" r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>102</v>
       </c>
@@ -2541,7 +2617,7 @@
       </c>
       <c r="G97" s="2"/>
     </row>
-    <row ht="15.75" r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>98</v>
       </c>
@@ -2562,7 +2638,7 @@
       </c>
       <c r="G98" s="2"/>
     </row>
-    <row ht="15.75" r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2624,14 +2700,14 @@
       <c r="G103" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC4A950-02FB-4771-9093-D3B7699EE31D}">
-  <dimension ref="A1:G3"/>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC4A950-02FB-4771-9093-D3B7699EE31D}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F3"/>
@@ -2640,16 +2716,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2696,34 +2772,34 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
-  <dimension ref="A1:G3"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2770,13 +2846,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
-  <dimension ref="A1:D5"/>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -2784,9 +2860,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2836,12 +2912,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2850,10 +2926,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="102.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="102.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2867,7 +2943,7 @@
         <v>58</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>62</v>
       </c>
@@ -2879,14 +2955,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -2894,9 +2970,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2922,13 +2998,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -2936,9 +3012,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="107.0" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="107" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2964,14 +3040,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
-  <dimension ref="A1:G2"/>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
@@ -2980,16 +3056,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3016,13 +3092,84 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C76C6E-154C-4EE9-B021-C644C18DD456}">
   <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -3030,17 +3177,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3081,172 +3228,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F635368-BB2D-4072-8E80-91DBE792F8EF}">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" customWidth="true" width="13.5703125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
-  <dimension ref="A1:J2"/>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -3254,14 +3243,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3312,14 +3301,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3EA4CE-EDA7-4242-A743-BE83DBFF6070}">
-  <dimension ref="A1:G3"/>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3EA4CE-EDA7-4242-A743-BE83DBFF6070}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -3328,16 +3317,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3384,13 +3373,151 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F635368-BB2D-4072-8E80-91DBE792F8EF}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="13.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
@@ -3439,26 +3566,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
-  <dimension ref="A1:G7"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="7" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="7" width="9.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="7" width="8.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" style="7" width="9.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="7" width="47.28515625" collapsed="true"/>
-    <col min="7" max="16384" style="7" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.42578125" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="47.28515625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="7" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3506,10 +3633,10 @@
         <v>99</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -3526,13 +3653,13 @@
         <v>100</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -3546,7 +3673,7 @@
         <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>27</v>
@@ -3555,18 +3682,18 @@
         <v>83</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>27</v>
@@ -3577,39 +3704,19 @@
       <c r="E6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>84</v>
+      <c r="F6" s="13" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0C12BF-7E83-4532-A128-E57EBFF1BF2D}">
-  <dimension ref="A1:F2"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0C12BF-7E83-4532-A128-E57EBFF1BF2D}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -3617,8 +3724,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3638,7 +3745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -3656,14 +3763,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2DE816-A9A4-4743-BF9C-2DEBCA2D1E71}">
-  <dimension ref="A1:F2"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2DE816-A9A4-4743-BF9C-2DEBCA2D1E71}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -3671,7 +3778,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3691,7 +3798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -3709,13 +3816,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97167B2-7C0B-4E15-B189-0ACF08094BA1}">
-  <dimension ref="A1:F2"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97167B2-7C0B-4E15-B189-0ACF08094BA1}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -3740,7 +3847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -3758,13 +3865,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
-  <dimension ref="A1:H1048576"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -3772,11 +3879,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="75.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="6" max="7" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="75.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3802,7 +3909,7 @@
         <v>68</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>81</v>
       </c>
@@ -3932,51 +4039,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2" xr:uid="{F1DC5D16-654A-4D10-A0DA-C3EC9A9CD3AC}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F1DC5D16-654A-4D10-A0DA-C3EC9A9CD3AC}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF31050-A1CE-4806-A18B-82FAF036D110}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated TSEE and Quick responses
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,44 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DA76FC-9677-4651-B633-6C025050DD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{C4E34E0F-5FA2-4357-946F-0D33372E211E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}"/>
+    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="TPSEE" sheetId="1" r:id="rId1"/>
-    <sheet name="Location_Page_Search" sheetId="22" r:id="rId2"/>
-    <sheet name="Facebook" sheetId="20" r:id="rId3"/>
-    <sheet name="Display_Review" sheetId="9" r:id="rId4"/>
-    <sheet name="Bing" sheetId="8" r:id="rId5"/>
-    <sheet name="FilterOrder" sheetId="17" r:id="rId6"/>
-    <sheet name="FilterOrderBing" sheetId="18" r:id="rId7"/>
-    <sheet name="FilterOrderFacebook" sheetId="19" r:id="rId8"/>
-    <sheet name="Duplicate_Management" sheetId="7" r:id="rId9"/>
-    <sheet name="Results" sheetId="15" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId11"/>
-    <sheet name="New Filters" sheetId="21" r:id="rId12"/>
-    <sheet name="BingZoom" sheetId="14" r:id="rId13"/>
-    <sheet name="Zoom" sheetId="2" r:id="rId14"/>
-    <sheet name="Syndication" sheetId="10" r:id="rId15"/>
-    <sheet name="Syndication DTCManual" sheetId="11" r:id="rId16"/>
-    <sheet name="Syndication DTCAPI" sheetId="13" r:id="rId17"/>
-    <sheet name="SyndicationLPAD" sheetId="12" r:id="rId18"/>
-    <sheet name="PDF" sheetId="3" r:id="rId19"/>
-    <sheet name="SA_Filters" sheetId="4" r:id="rId20"/>
-    <sheet name="SA_Advanced_Filters" sheetId="5" r:id="rId21"/>
-    <sheet name="SA_Zoom" sheetId="16" r:id="rId22"/>
+    <sheet name="TPSEE" r:id="rId1" sheetId="1"/>
+    <sheet name="Location_Page_Search" r:id="rId2" sheetId="22"/>
+    <sheet name="Facebook" r:id="rId3" sheetId="20"/>
+    <sheet name="Display_Review" r:id="rId4" sheetId="9"/>
+    <sheet name="Bing" r:id="rId5" sheetId="8"/>
+    <sheet name="FilterOrder" r:id="rId6" sheetId="17"/>
+    <sheet name="FilterOrderBing" r:id="rId7" sheetId="18"/>
+    <sheet name="FilterOrderFacebook" r:id="rId8" sheetId="19"/>
+    <sheet name="Duplicate_Management" r:id="rId9" sheetId="7"/>
+    <sheet name="Results" r:id="rId10" sheetId="15"/>
+    <sheet name="Sheet1" r:id="rId11" sheetId="6"/>
+    <sheet name="New Filters" r:id="rId12" sheetId="21"/>
+    <sheet name="BingZoom" r:id="rId13" sheetId="14"/>
+    <sheet name="Zoom" r:id="rId14" sheetId="2"/>
+    <sheet name="Syndication" r:id="rId15" sheetId="10"/>
+    <sheet name="Syndication DTCManual" r:id="rId16" sheetId="11"/>
+    <sheet name="Syndication DTCAPI" r:id="rId17" sheetId="13"/>
+    <sheet name="SyndicationLPAD" r:id="rId18" sheetId="12"/>
+    <sheet name="PDF" r:id="rId19" sheetId="3"/>
+    <sheet name="SA_Filters" r:id="rId20" sheetId="4"/>
+    <sheet name="SA_Advanced_Filters" r:id="rId21" sheetId="5"/>
+    <sheet name="SA_Zoom" r:id="rId22" sheetId="16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="136">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -446,22 +446,29 @@
     <t>Search By Phone</t>
   </si>
   <si>
-    <t>9000230163</t>
-  </si>
-  <si>
-    <t>Toronto</t>
-  </si>
-  <si>
-    <t>55425</t>
-  </si>
-  <si>
-    <t>+1 703-310-6711</t>
+    <t>9990308856</t>
+  </si>
+  <si>
+    <t>10038</t>
+  </si>
+  <si>
+    <t>+1 646-895-6831</t>
+  </si>
+  <si>
+    <t>101 Maiden</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Chicago</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -540,45 +547,45 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -595,10 +602,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -633,7 +640,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -685,7 +692,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -796,21 +803,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -827,7 +834,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -879,28 +886,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -948,10 +955,10 @@
         <v>99</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -968,13 +975,13 @@
         <v>100</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -988,7 +995,7 @@
         <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>27</v>
@@ -997,18 +1004,18 @@
         <v>83</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row ht="15.75" r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>27</v>
@@ -1019,45 +1026,25 @@
       <c r="E6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>84</v>
+      <c r="F6" s="13" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF31050-A1CE-4806-A18B-82FAF036D110}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF31050-A1CE-4806-A18B-82FAF036D110}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1086,14 +1073,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56B39C1-E271-4AB9-B9CD-EE7AE8CA71C2}">
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A25" sqref="A25:E25"/>
@@ -1101,10 +1088,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="90.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="90.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1265,17 +1252,17 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73840A65-FD3F-4FC7-8FDF-F89283B3CCE3}">
-  <dimension ref="A1:J103"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73840A65-FD3F-4FC7-8FDF-F89283B3CCE3}">
+  <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F7"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94:F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,7 +1380,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>102</v>
       </c>
@@ -1543,7 +1530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>98</v>
       </c>
@@ -1718,7 +1705,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>102</v>
       </c>
@@ -1897,7 +1884,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>98</v>
       </c>
@@ -2093,7 +2080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>102</v>
       </c>
@@ -2280,7 +2267,7 @@
       </c>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>102</v>
       </c>
@@ -2466,7 +2453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>102</v>
       </c>
@@ -2617,7 +2604,7 @@
       </c>
       <c r="G97" s="2"/>
     </row>
-    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>98</v>
       </c>
@@ -2638,7 +2625,7 @@
       </c>
       <c r="G98" s="2"/>
     </row>
-    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2700,14 +2687,14 @@
       <c r="G103" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC4A950-02FB-4771-9093-D3B7699EE31D}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC4A950-02FB-4771-9093-D3B7699EE31D}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F3"/>
@@ -2772,13 +2759,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C149A45-147A-4908-8AC2-DFFA5E3623E7}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -2786,7 +2773,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2846,13 +2833,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE83B1A1-2185-46E9-889B-398CF2C8D1EA}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -2860,9 +2847,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2912,12 +2899,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24410FF7-85D5-4227-A8AE-50DEA4701ACD}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2926,10 +2913,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="102.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="102.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2943,7 +2930,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>62</v>
       </c>
@@ -2955,14 +2942,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB44C4C-5432-437C-8705-E7CF64F0D75A}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -2970,9 +2957,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2998,13 +2985,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7ABE9-23D1-483E-B366-FA33B4CC2FB7}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -3012,9 +2999,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="107" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="107.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3040,14 +3027,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAB2C39-A780-44AF-8C3B-74F65247F33B}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
@@ -3092,30 +3079,30 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C76C6E-154C-4EE9-B021-C644C18DD456}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C76C6E-154C-4EE9-B021-C644C18DD456}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>123</v>
       </c>
@@ -3138,7 +3125,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>130</v>
       </c>
@@ -3146,30 +3133,30 @@
         <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G2" t="s">
-        <v>133</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2E35A7-13BB-4D66-BA23-E45FA9F5A588}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -3177,17 +3164,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3228,14 +3215,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E6707-7C93-426E-94F9-3A25A2415CB9}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -3243,14 +3230,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3301,14 +3288,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3EA4CE-EDA7-4242-A743-BE83DBFF6070}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3EA4CE-EDA7-4242-A743-BE83DBFF6070}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -3373,13 +3360,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F635368-BB2D-4072-8E80-91DBE792F8EF}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F635368-BB2D-4072-8E80-91DBE792F8EF}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F6"/>
@@ -3387,7 +3374,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" customWidth="true" width="13.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3490,7 +3477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>98</v>
       </c>
@@ -3511,13 +3498,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99D0056-9038-4B45-96BE-820C8A519FB7}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
@@ -3566,13 +3553,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245207A1-BB15-4AA9-AB10-62BB034F1692}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F6"/>
@@ -3580,12 +3567,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.42578125" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="47.28515625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="7" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="7" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="7" width="9.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="7" width="8.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" style="7" width="9.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="7" width="47.28515625" collapsed="true"/>
+    <col min="7" max="16384" style="7" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3688,7 +3675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>98</v>
       </c>
@@ -3709,14 +3696,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0C12BF-7E83-4532-A128-E57EBFF1BF2D}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0C12BF-7E83-4532-A128-E57EBFF1BF2D}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -3724,8 +3711,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3745,7 +3732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -3763,14 +3750,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2DE816-A9A4-4743-BF9C-2DEBCA2D1E71}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2DE816-A9A4-4743-BF9C-2DEBCA2D1E71}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -3778,7 +3765,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3798,7 +3785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -3816,13 +3803,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97167B2-7C0B-4E15-B189-0ACF08094BA1}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97167B2-7C0B-4E15-B189-0ACF08094BA1}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -3847,7 +3834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -3865,13 +3852,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
-  <dimension ref="A1:G1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66296A9-7A5C-4ED7-A4A1-E7DD7300B70D}">
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -3879,11 +3866,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="75.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="75.7109375" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3909,7 +3896,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>81</v>
       </c>
@@ -4039,9 +4026,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{F1DC5D16-654A-4D10-A0DA-C3EC9A9CD3AC}"/>
+    <hyperlink r:id="rId1" ref="B2" xr:uid="{F1DC5D16-654A-4D10-A0DA-C3EC9A9CD3AC}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated filters for TSEE Regression-Beta
</commit_message>
<xml_diff>
--- a/data/Filter.xlsx
+++ b/data/Filter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{C4E34E0F-5FA2-4357-946F-0D33372E211E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A8110932-DC6F-4A10-AE74-B6E193F09839}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{8A6A3122-5A59-4742-9374-8B4B8D56E6ED}" yWindow="-120"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="134">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -425,27 +425,6 @@
     <t>Aurify Brands - Date Filter - Location Level</t>
   </si>
   <si>
-    <t>Search By Location</t>
-  </si>
-  <si>
-    <t>Search By Name</t>
-  </si>
-  <si>
-    <t>Search By Address</t>
-  </si>
-  <si>
-    <t>Search By City</t>
-  </si>
-  <si>
-    <t>Search By State</t>
-  </si>
-  <si>
-    <t>Search By Postal Code</t>
-  </si>
-  <si>
-    <t>Search By Phone</t>
-  </si>
-  <si>
     <t>9990308856</t>
   </si>
   <si>
@@ -462,6 +441,21 @@
   </si>
   <si>
     <t>Chicago</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>St/Prov/Region</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
 </sst>
 </file>
@@ -894,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3AEA1-2378-4CC5-8688-3FA41A2FBF10}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F6"/>
+      <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,10 +949,10 @@
         <v>99</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -975,13 +969,13 @@
         <v>100</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -995,7 +989,7 @@
         <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>27</v>
@@ -1004,18 +998,18 @@
         <v>83</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row ht="15.75" r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>27</v>
@@ -1026,8 +1020,28 @@
       <c r="E6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>90</v>
+      <c r="F6" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1261,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73840A65-FD3F-4FC7-8FDF-F89283B3CCE3}">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:F98"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3087,9 +3101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C76C6E-154C-4EE9-B021-C644C18DD456}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3104,48 +3116,48 @@
   <sheetData>
     <row customFormat="1" r="1" s="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>123</v>
+        <v>40</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>126</v>
+        <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row ht="15.75" r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
         <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>